<commit_message>
Generate output as readable xlsx.
Added to final query some condition, that side-changing duplicates are excluded.

And write only text, and not node information into that df.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
   <si>
     <t>arg1</t>
   </si>
@@ -41,46 +41,106 @@
     <t>pred4</t>
   </si>
   <si>
-    <t>(_214:Expression {id: '33', s_id: '8', text: 'of the latter'})</t>
-  </si>
-  <si>
-    <t>(_213:Expression {id: '35', s_id: '8', text: 'of the former Man'})</t>
-  </si>
-  <si>
-    <t>(_219:Expression {id: '28', s_id: '8', text: 'Examples of the former Man , Ox , Runs , Wins'})</t>
-  </si>
-  <si>
-    <t>(_220:Expression {id: '23', s_id: '8', text: 'Examples of the latter ,'})</t>
-  </si>
-  <si>
-    <t>(_309:Expression {id: '32', s_id: '8', text: 'Examples of the latter'})</t>
-  </si>
-  <si>
-    <t>(_308:Expression {id: '34', s_id: '8', text: 'Examples of the former Man'})</t>
-  </si>
-  <si>
-    <t>(_312:Expression {id: '36', s_id: '8', text: 'Examples of the former are such expressions as Man , Ox , Runs , Wins'})</t>
-  </si>
-  <si>
-    <t>(_313:Expression {id: '37', s_id: '8', text: 'Examples of the latter are such expressions as Themanruns , Themanwins , .'})</t>
-  </si>
-  <si>
-    <t>(_216:Expression {id: '15', s_id: '8', text: 'such expressions as Themanruns'})</t>
-  </si>
-  <si>
-    <t>(_215:Expression {id: '20', s_id: '8', text: 'such expressions as'})</t>
-  </si>
-  <si>
-    <t>(_311:Expression {id: '12', s_id: '8', text: 'Examples of the latter are such expressions as Themanruns'})</t>
-  </si>
-  <si>
-    <t>(_310:Expression {id: '17', s_id: '8', text: 'Examples of the former are such expressions as Man'})</t>
-  </si>
-  <si>
-    <t>(_218:Expression {id: '26', s_id: '8', text: 'Themanruns , Themanwins'})</t>
-  </si>
-  <si>
-    <t>(_217:Expression {id: '31', s_id: '8', text: 'Man , Ox , Runs , Wins'})</t>
+    <t>the definition corresponding with the name</t>
+  </si>
+  <si>
+    <t>both the name and the definition answering to the name in common</t>
+  </si>
+  <si>
+    <t>they</t>
+  </si>
+  <si>
+    <t>it</t>
+  </si>
+  <si>
+    <t>Things are said to be named Equivocally when , though they have a common name , the definition corresponding with the name differs for each .</t>
+  </si>
+  <si>
+    <t>On the other hand , things are said to be named Univocally which have both the name and the definition answering to the name in common .</t>
+  </si>
+  <si>
+    <t>though they have a common name</t>
+  </si>
+  <si>
+    <t>Things are said to be named Derivatively , which derive their name from some other name , but differ from it in termination .</t>
+  </si>
+  <si>
+    <t>which</t>
+  </si>
+  <si>
+    <t>which have both the name answering to the name in common</t>
+  </si>
+  <si>
+    <t>to be which derive their name from some other name</t>
+  </si>
+  <si>
+    <t>the grammarian</t>
+  </si>
+  <si>
+    <t>Thus the grammarian derives his name from the word Grammar</t>
+  </si>
+  <si>
+    <t>their name</t>
+  </si>
+  <si>
+    <t>his name</t>
+  </si>
+  <si>
+    <t>Thus , the grammarian derives his name from the word Grammar , and the courageous man from the word Courage .</t>
+  </si>
+  <si>
+    <t>claim</t>
+  </si>
+  <si>
+    <t>Thus , a real man and a figure in a picture can both lay claim to the name Animal , yet these are equivocally so named , for , though they have a common name , the definition corresponding with the name differs for each .</t>
+  </si>
+  <si>
+    <t>the name</t>
+  </si>
+  <si>
+    <t>the word Grammar</t>
+  </si>
+  <si>
+    <t>of the former Man</t>
+  </si>
+  <si>
+    <t>of the latter</t>
+  </si>
+  <si>
+    <t>Examples of the latter ,</t>
+  </si>
+  <si>
+    <t>Examples of the former Man , Ox , Runs , Wins</t>
+  </si>
+  <si>
+    <t>Examples of the former Man</t>
+  </si>
+  <si>
+    <t>Examples of the latter</t>
+  </si>
+  <si>
+    <t>Examples of the latter are such expressions as Themanruns , Themanwins , .</t>
+  </si>
+  <si>
+    <t>Examples of the former are such expressions as Man , Ox , Runs , Wins</t>
+  </si>
+  <si>
+    <t>such expressions as</t>
+  </si>
+  <si>
+    <t>such expressions as Themanruns</t>
+  </si>
+  <si>
+    <t>Examples of the former are such expressions as Man</t>
+  </si>
+  <si>
+    <t>Examples of the latter are such expressions as Themanruns</t>
+  </si>
+  <si>
+    <t>Man , Ox , Runs , Wins</t>
+  </si>
+  <si>
+    <t>Themanruns , Themanwins</t>
   </si>
 </sst>
 </file>
@@ -429,7 +489,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,28 +557,28 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -526,28 +586,28 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" t="s">
-        <v>14</v>
-      </c>
       <c r="I4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -555,28 +615,28 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="I5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -584,28 +644,28 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
         <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
         <v>15</v>
       </c>
-      <c r="G6" t="s">
-        <v>14</v>
-      </c>
       <c r="H6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I6" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -613,28 +673,28 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
         <v>21</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>9</v>
       </c>
-      <c r="E7" t="s">
-        <v>8</v>
-      </c>
       <c r="F7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" t="s">
         <v>15</v>
       </c>
-      <c r="G7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>13</v>
-      </c>
-      <c r="I7" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -642,28 +702,28 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
         <v>21</v>
       </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" t="s">
         <v>15</v>
       </c>
-      <c r="H8" t="s">
-        <v>18</v>
-      </c>
       <c r="I8" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -671,28 +731,115 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="E9" t="s">
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="F9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" t="s">
-        <v>13</v>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished working on the parallelistic-in different ways elliptical-correlating testcase
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -15,19 +15,71 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+  <si>
+    <t>arg1</t>
+  </si>
+  <si>
+    <t>arg2</t>
+  </si>
+  <si>
+    <t>arg3</t>
+  </si>
+  <si>
+    <t>arg4</t>
+  </si>
+  <si>
+    <t>pred1</t>
+  </si>
+  <si>
+    <t>pred2</t>
+  </si>
+  <si>
+    <t>pred3</t>
+  </si>
+  <si>
+    <t>pred4</t>
+  </si>
+  <si>
+    <t>to the name</t>
+  </si>
+  <si>
+    <t>their name</t>
+  </si>
+  <si>
+    <t>common</t>
+  </si>
+  <si>
+    <t>it</t>
+  </si>
+  <si>
+    <t>On the other hand , things are said to be named Univocally which have both the name and the definition answering to the name in common .</t>
+  </si>
+  <si>
+    <t>Things are said to be named Derivatively , which derive their name from some other name , but differ from it in termination .</t>
+  </si>
+  <si>
+    <t>both the name answering to the name in common</t>
+  </si>
+  <si>
+    <t>to be which derive their name from some other name</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -38,7 +90,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -46,12 +98,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -349,14 +411,70 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Build subjects and aspects with coreference resolution
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
   <si>
     <t>arg1</t>
   </si>
@@ -41,28 +41,67 @@
     <t>pred4</t>
   </si>
   <si>
-    <t>to the name</t>
+    <t>things</t>
+  </si>
+  <si>
+    <t>Things</t>
+  </si>
+  <si>
+    <t>both the name and the definition answering to the name in common</t>
   </si>
   <si>
     <t>their name</t>
   </si>
   <si>
+    <t>On the other hand , things are said to be named Univocally which have both the name and the definition answering to the name in common .</t>
+  </si>
+  <si>
+    <t>Things are said to be named Derivatively , which derive their name from some other name , but differ from it in termination .</t>
+  </si>
+  <si>
+    <t>which have both the name answering to the name in common</t>
+  </si>
+  <si>
+    <t>to be which derive their name from some other name</t>
+  </si>
+  <si>
+    <t>both the name answering to the name in common</t>
+  </si>
+  <si>
+    <t>the other hand</t>
+  </si>
+  <si>
+    <t>some other name</t>
+  </si>
+  <si>
+    <t>the name</t>
+  </si>
+  <si>
+    <t>a common name</t>
+  </si>
+  <si>
+    <t>though they have a common name</t>
+  </si>
+  <si>
+    <t>Things are said to be named Equivocally when the definition corresponding with the name differs for each</t>
+  </si>
+  <si>
+    <t>Things are said to be named Derivatively</t>
+  </si>
+  <si>
+    <t>when the definition corresponding with the name differs for each</t>
+  </si>
+  <si>
+    <t>Things are differ from it in termination</t>
+  </si>
+  <si>
+    <t>the definition corresponding with the name</t>
+  </si>
+  <si>
+    <t>Things are said to be named Equivocally when , though they have a common name , the definition corresponding with the name differs for each .</t>
+  </si>
+  <si>
     <t>common</t>
-  </si>
-  <si>
-    <t>it</t>
-  </si>
-  <si>
-    <t>On the other hand , things are said to be named Univocally which have both the name and the definition answering to the name in common .</t>
-  </si>
-  <si>
-    <t>Things are said to be named Derivatively , which derive their name from some other name , but differ from it in termination .</t>
-  </si>
-  <si>
-    <t>both the name answering to the name in common</t>
-  </si>
-  <si>
-    <t>to be which derive their name from some other name</t>
   </si>
 </sst>
 </file>
@@ -411,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,6 +513,876 @@
         <v>15</v>
       </c>
     </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" t="s">
+        <v>12</v>
+      </c>
+      <c r="I21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" t="s">
+        <v>27</v>
+      </c>
+      <c r="G24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" t="s">
+        <v>27</v>
+      </c>
+      <c r="G25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" t="s">
+        <v>24</v>
+      </c>
+      <c r="I25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G26" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" t="s">
+        <v>24</v>
+      </c>
+      <c r="I26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G27" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" t="s">
+        <v>27</v>
+      </c>
+      <c r="G28" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28" t="s">
+        <v>26</v>
+      </c>
+      <c r="I28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" t="s">
+        <v>27</v>
+      </c>
+      <c r="G29" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29" t="s">
+        <v>21</v>
+      </c>
+      <c r="I29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30" t="s">
+        <v>27</v>
+      </c>
+      <c r="G30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" t="s">
+        <v>21</v>
+      </c>
+      <c r="I30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" t="s">
+        <v>27</v>
+      </c>
+      <c r="G31" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31" t="s">
+        <v>20</v>
+      </c>
+      <c r="I31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" t="s">
+        <v>27</v>
+      </c>
+      <c r="G32" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" t="s">
+        <v>20</v>
+      </c>
+      <c r="I32" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>